<commit_message>
feat: sincronizar fechas reales de ALTA desde ANEXO A (diciembre 2025)
- Extraídas 75 fechas de ANEXO A (CLUB 738-31-DE-DICIEMBRE-2025_ANEXOS A, B Y C.xlsx)
- Sincronizadas 286 fechas en FUENTE_DE_VERDAD (columnas A-E y I)
- Fechas reales por socio:
  • Ricardo Fernández: 2007-07-26
  • José Lizárraga: 2021-10-02
  • Adolfo Xacur: 2009-01-09
  • Remigio Aguilar: 2021-07-03
  • Manuel Chaidez: 2009-09-10
  • ... y 70 más
- Reportes RELACIÓN y ANEXO A regenerados
</commit_message>
<xml_diff>
--- a/data/referencias/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/data/referencias/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -484,8 +484,8 @@
       <c r="G2" t="str">
         <v>richfegas@icloud.com</v>
       </c>
-      <c r="H2">
-        <v>25568.750454722223</v>
+      <c r="H2" t="str">
+        <v>2007-07-26</v>
       </c>
       <c r="I2" t="str">
         <v>CALLE 44 No. 438 x 21 y 23</v>
@@ -543,8 +543,8 @@
       <c r="G3" t="str">
         <v>richfegas@icloud.com</v>
       </c>
-      <c r="H3">
-        <v>25568.750454722223</v>
+      <c r="H3" t="str">
+        <v>2007-07-26</v>
       </c>
       <c r="I3" t="str">
         <v>CALLE 44 No. 438 x 21 y 23</v>
@@ -602,8 +602,8 @@
       <c r="G4" t="str">
         <v>richfegas@icloud.com</v>
       </c>
-      <c r="H4">
-        <v>25568.750454722223</v>
+      <c r="H4" t="str">
+        <v>2007-07-26</v>
       </c>
       <c r="I4" t="str">
         <v>CALLE 44 No. 438 x 21 y 23</v>
@@ -661,8 +661,8 @@
       <c r="G5" t="str">
         <v>richfegas@icloud.com</v>
       </c>
-      <c r="H5">
-        <v>25568.750454722223</v>
+      <c r="H5" t="str">
+        <v>2007-07-26</v>
       </c>
       <c r="I5" t="str">
         <v>CALLE 44 No. 438 x 21 y 23</v>
@@ -720,8 +720,8 @@
       <c r="G6" t="str">
         <v>jacintolizarraga@hotmail.com</v>
       </c>
-      <c r="H6">
-        <v>25568.750514699073</v>
+      <c r="H6" t="str">
+        <v>2021-10-02</v>
       </c>
       <c r="I6" t="str">
         <v>CALLE 25 x 22 y 24 No. 319</v>
@@ -779,8 +779,8 @@
       <c r="G7" t="str">
         <v>jacintolizarraga@hotmail.com</v>
       </c>
-      <c r="H7">
-        <v>25568.750514699073</v>
+      <c r="H7" t="str">
+        <v>2021-10-02</v>
       </c>
       <c r="I7" t="str">
         <v>CALLE 25 x 22 y 24 No. 319</v>
@@ -838,8 +838,8 @@
       <c r="G8" t="str">
         <v>jacintolizarraga@hotmail.com</v>
       </c>
-      <c r="H8">
-        <v>25568.750514699073</v>
+      <c r="H8" t="str">
+        <v>2021-10-02</v>
       </c>
       <c r="I8" t="str">
         <v>CALLE 25 x 22 y 24 No. 319</v>
@@ -897,8 +897,8 @@
       <c r="G9" t="str">
         <v>jacintolizarraga@hotmail.com</v>
       </c>
-      <c r="H9">
-        <v>25568.750514699073</v>
+      <c r="H9" t="str">
+        <v>2021-10-02</v>
       </c>
       <c r="I9" t="str">
         <v>CALLE 25 x 22 y 24 No. 319</v>
@@ -956,8 +956,8 @@
       <c r="G10" t="str">
         <v>jacintolizarraga@hotmail.com</v>
       </c>
-      <c r="H10">
-        <v>25568.750514699073</v>
+      <c r="H10" t="str">
+        <v>2021-10-02</v>
       </c>
       <c r="I10" t="str">
         <v>CALLE 25 x 22 y 24 No. 319</v>
@@ -1015,8 +1015,8 @@
       <c r="G11" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H11">
-        <v>25568.75046090278</v>
+      <c r="H11" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I11" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1074,8 +1074,8 @@
       <c r="G12" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H12">
-        <v>25568.75046090278</v>
+      <c r="H12" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I12" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1133,8 +1133,8 @@
       <c r="G13" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H13">
-        <v>25568.75046090278</v>
+      <c r="H13" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I13" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1192,8 +1192,8 @@
       <c r="G14" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H14">
-        <v>25568.75046090278</v>
+      <c r="H14" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I14" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1251,8 +1251,8 @@
       <c r="G15" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H15">
-        <v>25568.75046090278</v>
+      <c r="H15" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I15" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1310,8 +1310,8 @@
       <c r="G16" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H16">
-        <v>25568.75046090278</v>
+      <c r="H16" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I16" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1369,8 +1369,8 @@
       <c r="G17" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H17">
-        <v>25568.75046090278</v>
+      <c r="H17" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I17" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1428,8 +1428,8 @@
       <c r="G18" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="H18">
-        <v>25568.75046090278</v>
+      <c r="H18" t="str">
+        <v>2009-01-09</v>
       </c>
       <c r="I18" t="str">
         <v>Calle 36-B No. 285 x 33 y 35</v>
@@ -1487,8 +1487,8 @@
       <c r="G19" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H19">
-        <v>25568.750513645835</v>
+      <c r="H19" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I19" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1546,8 +1546,8 @@
       <c r="G20" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H20">
-        <v>25568.750513645835</v>
+      <c r="H20" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I20" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1605,8 +1605,8 @@
       <c r="G21" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H21">
-        <v>25568.750513645835</v>
+      <c r="H21" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I21" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1664,8 +1664,8 @@
       <c r="G22" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H22">
-        <v>25568.750513645835</v>
+      <c r="H22" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I22" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1723,8 +1723,8 @@
       <c r="G23" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H23">
-        <v>25568.750513645835</v>
+      <c r="H23" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I23" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1782,8 +1782,8 @@
       <c r="G24" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H24">
-        <v>25568.750513645835</v>
+      <c r="H24" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I24" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1841,8 +1841,8 @@
       <c r="G25" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H25">
-        <v>25568.750513645835</v>
+      <c r="H25" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I25" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1900,8 +1900,8 @@
       <c r="G26" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H26">
-        <v>25568.750513645835</v>
+      <c r="H26" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I26" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -1959,8 +1959,8 @@
       <c r="G27" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H27">
-        <v>25568.750513645835</v>
+      <c r="H27" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I27" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -2018,8 +2018,8 @@
       <c r="G28" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="H28">
-        <v>25568.750513645835</v>
+      <c r="H28" t="str">
+        <v>2021-07-03</v>
       </c>
       <c r="I28" t="str">
         <v>Calle 20 No. 50 x 5 y 7</v>
@@ -2078,8 +2078,8 @@
       <c r="G29" t="str">
         <v>manuel.chaidez@valledelsur.com.mx</v>
       </c>
-      <c r="H29">
-        <v>25568.750463715278</v>
+      <c r="H29" t="str">
+        <v>2009-09-10</v>
       </c>
       <c r="I29" t="str">
         <v>DOMICILIO CONOCIDO ANEXO 3 CERCA DE LA COCINA</v>
@@ -2137,8 +2137,8 @@
       <c r="G30" t="str">
         <v>manuel.chaidez@valledelsur.com.mx</v>
       </c>
-      <c r="H30">
-        <v>25568.750463715278</v>
+      <c r="H30" t="str">
+        <v>2009-09-10</v>
       </c>
       <c r="I30" t="str">
         <v>DOMICILIO CONOCIDO ANEXO 3 CERCA DE LA COCINA</v>
@@ -2196,8 +2196,8 @@
       <c r="G31" t="str">
         <v>manuel.chaidez@valledelsur.com.mx</v>
       </c>
-      <c r="H31">
-        <v>25568.750463715278</v>
+      <c r="H31" t="str">
+        <v>2009-09-10</v>
       </c>
       <c r="I31" t="str">
         <v>DOMICILIO CONOCIDO ANEXO 3 CERCA DE LA COCINA</v>
@@ -2255,8 +2255,8 @@
       <c r="G32" t="str">
         <v>manuel.chaidez@valledelsur.com.mx</v>
       </c>
-      <c r="H32">
-        <v>25568.750463715278</v>
+      <c r="H32" t="str">
+        <v>2009-09-10</v>
       </c>
       <c r="I32" t="str">
         <v>DOMICILIO CONOCIDO ANEXO 3 CERCA DE LA COCINA</v>
@@ -2314,8 +2314,8 @@
       <c r="G33" t="str">
         <v>manuel.chaidez@valledelsur.com.mx</v>
       </c>
-      <c r="H33">
-        <v>25568.750463715278</v>
+      <c r="H33" t="str">
+        <v>2009-09-10</v>
       </c>
       <c r="I33" t="str">
         <v>DOMICILIO CONOCIDO ANEXO 3 CERCA DE LA COCINA</v>
@@ -2373,8 +2373,8 @@
       <c r="G34" t="str">
         <v>talleresmonforte@hotmail.com</v>
       </c>
-      <c r="H34">
-        <v>25568.750464675926</v>
+      <c r="H34" t="str">
+        <v>2009-12-01</v>
       </c>
       <c r="I34" t="str">
         <v>CALLE 33 No. 331 x 18 y 20</v>
@@ -2432,8 +2432,8 @@
       <c r="G35" t="str">
         <v>talleresmonforte@hotmail.com</v>
       </c>
-      <c r="H35">
-        <v>25568.750464675926</v>
+      <c r="H35" t="str">
+        <v>2009-12-01</v>
       </c>
       <c r="I35" t="str">
         <v>CALLE 33 No. 331 x 18 y 20</v>
@@ -2491,8 +2491,8 @@
       <c r="G36" t="str">
         <v>talleresmonforte@hotmail.com</v>
       </c>
-      <c r="H36">
-        <v>25568.750464675926</v>
+      <c r="H36" t="str">
+        <v>2009-12-01</v>
       </c>
       <c r="I36" t="str">
         <v>CALLE 33 No. 331 x 18 y 20</v>
@@ -2550,8 +2550,8 @@
       <c r="G37" t="str">
         <v>talleresmonforte@hotmail.com</v>
       </c>
-      <c r="H37">
-        <v>25568.750464675926</v>
+      <c r="H37" t="str">
+        <v>2009-12-01</v>
       </c>
       <c r="I37" t="str">
         <v>CALLE 33 No. 331 x 18 y 20</v>
@@ -2609,8 +2609,8 @@
       <c r="G38" t="str">
         <v>talleresmonforte@hotmail.com</v>
       </c>
-      <c r="H38">
-        <v>25568.750464675926</v>
+      <c r="H38" t="str">
+        <v>2009-12-01</v>
       </c>
       <c r="I38" t="str">
         <v>CALLE 33 No. 331 x 18 y 20</v>
@@ -2668,8 +2668,8 @@
       <c r="G39" t="str">
         <v>talleresmonforte@hotmail.com</v>
       </c>
-      <c r="H39">
-        <v>25568.750464675926</v>
+      <c r="H39" t="str">
+        <v>2009-12-01</v>
       </c>
       <c r="I39" t="str">
         <v>CALLE 33 No. 331 x 18 y 20</v>
@@ -2727,8 +2727,8 @@
       <c r="G40" t="str">
         <v>talleresmonforte@hotmail.com</v>
       </c>
-      <c r="H40">
-        <v>25568.750464675926</v>
+      <c r="H40" t="str">
+        <v>2009-12-01</v>
       </c>
       <c r="I40" t="str">
         <v>CALLE 33 No. 331 x 18 y 20</v>
@@ -2786,8 +2786,8 @@
       <c r="G41" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H41">
-        <v>25568.750468194445</v>
+      <c r="H41" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I41" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -2845,8 +2845,8 @@
       <c r="G42" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H42">
-        <v>25568.750468194445</v>
+      <c r="H42" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I42" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -2904,8 +2904,8 @@
       <c r="G43" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H43">
-        <v>25568.750468194445</v>
+      <c r="H43" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I43" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -2963,8 +2963,8 @@
       <c r="G44" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H44">
-        <v>25568.750468194445</v>
+      <c r="H44" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I44" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -3022,8 +3022,8 @@
       <c r="G45" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H45">
-        <v>25568.750468194445</v>
+      <c r="H45" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I45" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -3081,8 +3081,8 @@
       <c r="G46" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H46">
-        <v>25568.750468194445</v>
+      <c r="H46" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I46" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -3140,8 +3140,8 @@
       <c r="G47" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H47">
-        <v>25568.750468194445</v>
+      <c r="H47" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I47" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -3199,8 +3199,8 @@
       <c r="G48" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H48">
-        <v>25568.750468194445</v>
+      <c r="H48" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I48" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -3258,8 +3258,8 @@
       <c r="G49" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H49">
-        <v>25568.750468194445</v>
+      <c r="H49" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I49" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -3317,8 +3317,8 @@
       <c r="G50" t="str">
         <v>recosadecv@prodigy.net.mx</v>
       </c>
-      <c r="H50">
-        <v>25568.750468194445</v>
+      <c r="H50" t="str">
+        <v>2010-10-02</v>
       </c>
       <c r="I50" t="str">
         <v>AV. EUGENIO ECHEVERRÍA CASTELLOT No. 37 ENTRE 36 Y 38</v>
@@ -3376,8 +3376,8 @@
       <c r="G51" t="str">
         <v>jordan910@hotmail.com</v>
       </c>
-      <c r="H51">
-        <v>25568.750470266205</v>
+      <c r="H51" t="str">
+        <v>2011-03-29</v>
       </c>
       <c r="I51" t="str">
         <v>CALLE 16-B No. 225 x 39-B y 39-F</v>
@@ -3435,8 +3435,8 @@
       <c r="G52" t="str">
         <v>jordan910@hotmail.com</v>
       </c>
-      <c r="H52">
-        <v>25568.750470266205</v>
+      <c r="H52" t="str">
+        <v>2011-03-29</v>
       </c>
       <c r="I52" t="str">
         <v>CALLE 16-B No. 225 x 39-B y 39-F</v>
@@ -3494,8 +3494,8 @@
       <c r="G53" t="str">
         <v>jordan910@hotmail.com</v>
       </c>
-      <c r="H53">
-        <v>25568.750470266205</v>
+      <c r="H53" t="str">
+        <v>2011-03-29</v>
       </c>
       <c r="I53" t="str">
         <v>CALLE 16-B No. 225 x 39-B y 39-F</v>
@@ -3553,8 +3553,8 @@
       <c r="G54" t="str">
         <v>jordan910@hotmail.com</v>
       </c>
-      <c r="H54">
-        <v>25568.750470266205</v>
+      <c r="H54" t="str">
+        <v>2011-03-29</v>
       </c>
       <c r="I54" t="str">
         <v>CALLE 16-B No. 225 x 39-B y 39-F</v>
@@ -3612,8 +3612,8 @@
       <c r="G55" t="str">
         <v>jorgedawn@prodigy.net.mx</v>
       </c>
-      <c r="H55">
-        <v>25568.750514537038</v>
+      <c r="H55" t="str">
+        <v>2021-09-18</v>
       </c>
       <c r="I55" t="str">
         <v>CALLE 47-C S/N x 2-A y 4</v>
@@ -3671,8 +3671,8 @@
       <c r="G56" t="str">
         <v>jorgedawn@prodigy.net.mx</v>
       </c>
-      <c r="H56">
-        <v>25568.750514537038</v>
+      <c r="H56" t="str">
+        <v>2021-09-18</v>
       </c>
       <c r="I56" t="str">
         <v>CALLE 47-C S/N x 2-A y 4</v>
@@ -3730,8 +3730,8 @@
       <c r="G57" t="str">
         <v>jorgedawn@prodigy.net.mx</v>
       </c>
-      <c r="H57">
-        <v>25568.750514537038</v>
+      <c r="H57" t="str">
+        <v>2021-09-18</v>
       </c>
       <c r="I57" t="str">
         <v>CALLE 47-C S/N x 2-A y 4</v>
@@ -3789,8 +3789,8 @@
       <c r="G58" t="str">
         <v>jorgedawn@prodigy.net.mx</v>
       </c>
-      <c r="H58">
-        <v>25568.750514537038</v>
+      <c r="H58" t="str">
+        <v>2021-09-18</v>
       </c>
       <c r="I58" t="str">
         <v>CALLE 47-C S/N x 2-A y 4</v>
@@ -3848,8 +3848,8 @@
       <c r="G59" t="str">
         <v>jorgedawn@prodigy.net.mx</v>
       </c>
-      <c r="H59">
-        <v>25568.750514537038</v>
+      <c r="H59" t="str">
+        <v>2021-09-18</v>
       </c>
       <c r="I59" t="str">
         <v>CALLE 47-C S/N x 2-A y 4</v>
@@ -3907,8 +3907,8 @@
       <c r="G60" t="str">
         <v>jorgedawn@prodigy.net.mx</v>
       </c>
-      <c r="H60">
-        <v>25568.750514537038</v>
+      <c r="H60" t="str">
+        <v>2021-09-18</v>
       </c>
       <c r="I60" t="str">
         <v>CALLE 47-C S/N x 2-A y 4</v>
@@ -3966,8 +3966,8 @@
       <c r="G61" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H61">
-        <v>25568.750471631945</v>
+      <c r="H61" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I61" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4025,8 +4025,8 @@
       <c r="G62" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H62">
-        <v>25568.750471631945</v>
+      <c r="H62" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I62" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4084,8 +4084,8 @@
       <c r="G63" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H63">
-        <v>25568.750471631945</v>
+      <c r="H63" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I63" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4143,8 +4143,8 @@
       <c r="G64" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H64">
-        <v>25568.750471631945</v>
+      <c r="H64" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I64" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4202,8 +4202,8 @@
       <c r="G65" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H65">
-        <v>25568.750471631945</v>
+      <c r="H65" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I65" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4261,8 +4261,8 @@
       <c r="G66" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H66">
-        <v>25568.750471631945</v>
+      <c r="H66" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I66" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4320,8 +4320,8 @@
       <c r="G67" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H67">
-        <v>25568.750471631945</v>
+      <c r="H67" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I67" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4379,8 +4379,8 @@
       <c r="G68" t="str">
         <v>ssg@santinelli.com.mx</v>
       </c>
-      <c r="H68">
-        <v>25568.750471631945</v>
+      <c r="H68" t="str">
+        <v>2011-07-26</v>
       </c>
       <c r="I68" t="str">
         <v>CALLE KANHA No. 85</v>
@@ -4438,8 +4438,8 @@
       <c r="G69" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H69">
-        <v>25568.750514502313</v>
+      <c r="H69" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I69" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4497,8 +4497,8 @@
       <c r="G70" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H70">
-        <v>25568.750514502313</v>
+      <c r="H70" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I70" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4556,8 +4556,8 @@
       <c r="G71" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H71">
-        <v>25568.750514502313</v>
+      <c r="H71" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I71" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4615,8 +4615,8 @@
       <c r="G72" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H72">
-        <v>25568.750514502313</v>
+      <c r="H72" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I72" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4674,8 +4674,8 @@
       <c r="G73" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H73">
-        <v>25568.750514502313</v>
+      <c r="H73" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I73" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4733,8 +4733,8 @@
       <c r="G74" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H74">
-        <v>25568.750514502313</v>
+      <c r="H74" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I74" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4792,8 +4792,8 @@
       <c r="G75" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H75">
-        <v>25568.750514502313</v>
+      <c r="H75" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I75" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4851,8 +4851,8 @@
       <c r="G76" t="str">
         <v>cc@secure.mx</v>
       </c>
-      <c r="H76">
-        <v>25568.750514502313</v>
+      <c r="H76" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I76" t="str">
         <v>PASEO DE LOS AHUEHUETES No. 874 entre B NÍSPEROS Y B CASTAÑOS</v>
@@ -4910,8 +4910,8 @@
       <c r="G77" t="str">
         <v>al3xrivas@gmail.com</v>
       </c>
-      <c r="H77">
-        <v>25568.750514502313</v>
+      <c r="H77" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I77" t="str">
         <v>CALLE 42 No. 194-A x 35 y 37</v>
@@ -4969,8 +4969,8 @@
       <c r="G78" t="str">
         <v>al3xrivas@gmail.com</v>
       </c>
-      <c r="H78">
-        <v>25568.750514502313</v>
+      <c r="H78" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I78" t="str">
         <v>CALLE 42 No. 194-A x 35 y 37</v>
@@ -5028,8 +5028,8 @@
       <c r="G79" t="str">
         <v>al3xrivas@gmail.com</v>
       </c>
-      <c r="H79">
-        <v>25568.750514502313</v>
+      <c r="H79" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I79" t="str">
         <v>CALLE 42 No. 194-A x 35 y 37</v>
@@ -5087,8 +5087,8 @@
       <c r="G80" t="str">
         <v>al3xrivas@gmail.com</v>
       </c>
-      <c r="H80">
-        <v>25568.750514502313</v>
+      <c r="H80" t="str">
+        <v>2021-09-15</v>
       </c>
       <c r="I80" t="str">
         <v>CALLE 42 No. 194-A x 35 y 37</v>
@@ -5146,8 +5146,8 @@
       <c r="G81" t="str">
         <v>jvtl@hotmail.com</v>
       </c>
-      <c r="H81">
-        <v>25568.75047545139</v>
+      <c r="H81" t="str">
+        <v>2012-06-20</v>
       </c>
       <c r="I81" t="str">
         <v>CALLE 32 NÚM. 232 B x 37 y 45 DIAGONAL</v>
@@ -5205,8 +5205,8 @@
       <c r="G82" t="str">
         <v>jvtl@hotmail.com</v>
       </c>
-      <c r="H82">
-        <v>25568.75047545139</v>
+      <c r="H82" t="str">
+        <v>2012-06-20</v>
       </c>
       <c r="I82" t="str">
         <v>CALLE 32 NÚM. 232 B x 37 y 45 DIAGONAL</v>
@@ -5264,8 +5264,8 @@
       <c r="G83" t="str">
         <v>jvtl@hotmail.com</v>
       </c>
-      <c r="H83">
-        <v>25568.75047545139</v>
+      <c r="H83" t="str">
+        <v>2012-06-20</v>
       </c>
       <c r="I83" t="str">
         <v>CALLE 32 NÚM. 232 B x 37 y 45 DIAGONAL</v>
@@ -5323,8 +5323,8 @@
       <c r="G84" t="str">
         <v>monfo87_@hotmail.com</v>
       </c>
-      <c r="H84">
-        <v>25568.75047576389</v>
+      <c r="H84" t="str">
+        <v>2012-07-17</v>
       </c>
       <c r="I84" t="str">
         <v>CALLE 35 No. 331 x 18 y 20</v>
@@ -5382,8 +5382,8 @@
       <c r="G85" t="str">
         <v>monfo87_@hotmail.com</v>
       </c>
-      <c r="H85">
-        <v>25568.75047576389</v>
+      <c r="H85" t="str">
+        <v>2012-07-17</v>
       </c>
       <c r="I85" t="str">
         <v>CALLE 35 No. 331 x 18 y 20</v>
@@ -5441,8 +5441,8 @@
       <c r="G86" t="str">
         <v>monfo87_@hotmail.com</v>
       </c>
-      <c r="H86">
-        <v>25568.75047576389</v>
+      <c r="H86" t="str">
+        <v>2012-07-17</v>
       </c>
       <c r="I86" t="str">
         <v>CALLE 35 No. 331 x 18 y 20</v>
@@ -5500,8 +5500,8 @@
       <c r="G87" t="str">
         <v>monfo87_@hotmail.com</v>
       </c>
-      <c r="H87">
-        <v>25568.75047576389</v>
+      <c r="H87" t="str">
+        <v>2012-07-17</v>
       </c>
       <c r="I87" t="str">
         <v>CALLE 35 No. 331 x 18 y 20</v>
@@ -5559,8 +5559,8 @@
       <c r="G88" t="str">
         <v>monfo87_@hotmail.com</v>
       </c>
-      <c r="H88">
-        <v>25568.75047576389</v>
+      <c r="H88" t="str">
+        <v>2012-07-17</v>
       </c>
       <c r="I88" t="str">
         <v>CALLE 35 No. 331 x 18 y 20</v>
@@ -5618,8 +5618,8 @@
       <c r="G89" t="str">
         <v>jcb197624@hotmail.com</v>
       </c>
-      <c r="H89">
-        <v>25568.750476064815</v>
+      <c r="H89" t="str">
+        <v>2012-08-12</v>
       </c>
       <c r="I89" t="str">
         <v>CALLE 17-A No. 389 x 16-A y 16-B</v>
@@ -5677,8 +5677,8 @@
       <c r="G90" t="str">
         <v>jcb197624@hotmail.com</v>
       </c>
-      <c r="H90">
-        <v>25568.750476064815</v>
+      <c r="H90" t="str">
+        <v>2012-08-12</v>
       </c>
       <c r="I90" t="str">
         <v>CALLE 17-A No. 389 x 16-A y 16-B</v>
@@ -5736,8 +5736,8 @@
       <c r="G91" t="str">
         <v>jcb197624@hotmail.com</v>
       </c>
-      <c r="H91">
-        <v>25568.750476064815</v>
+      <c r="H91" t="str">
+        <v>2012-08-12</v>
       </c>
       <c r="I91" t="str">
         <v>CALLE 17-A No. 389 x 16-A y 16-B</v>
@@ -5795,8 +5795,8 @@
       <c r="G92" t="str">
         <v>jcb197624@hotmail.com</v>
       </c>
-      <c r="H92">
-        <v>25568.750476064815</v>
+      <c r="H92" t="str">
+        <v>2012-08-12</v>
       </c>
       <c r="I92" t="str">
         <v>CALLE 17-A No. 389 x 16-A y 16-B</v>
@@ -5854,8 +5854,8 @@
       <c r="G93" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H93">
-        <v>25568.750476597223</v>
+      <c r="H93" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I93" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -5913,8 +5913,8 @@
       <c r="G94" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H94">
-        <v>25568.750476597223</v>
+      <c r="H94" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I94" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -5972,8 +5972,8 @@
       <c r="G95" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H95">
-        <v>25568.750476597223</v>
+      <c r="H95" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I95" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6031,8 +6031,8 @@
       <c r="G96" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H96">
-        <v>25568.750476597223</v>
+      <c r="H96" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I96" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6090,8 +6090,8 @@
       <c r="G97" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H97">
-        <v>25568.750476597223</v>
+      <c r="H97" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I97" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6149,8 +6149,8 @@
       <c r="G98" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H98">
-        <v>25568.750476597223</v>
+      <c r="H98" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I98" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6208,8 +6208,8 @@
       <c r="G99" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H99">
-        <v>25568.750476597223</v>
+      <c r="H99" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I99" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6267,8 +6267,8 @@
       <c r="G100" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H100">
-        <v>25568.750476597223</v>
+      <c r="H100" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I100" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6326,8 +6326,8 @@
       <c r="G101" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H101">
-        <v>25568.750476597223</v>
+      <c r="H101" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I101" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6385,8 +6385,8 @@
       <c r="G102" t="str">
         <v>carlosgranja@gmail.com</v>
       </c>
-      <c r="H102">
-        <v>25568.750476597223</v>
+      <c r="H102" t="str">
+        <v>2012-09-27</v>
       </c>
       <c r="I102" t="str">
         <v>CALLE 35 No. 36 x 12 y 14</v>
@@ -6562,8 +6562,8 @@
       <c r="G105" t="str">
         <v>humh4@hotmail.com</v>
       </c>
-      <c r="H105">
-        <v>25568.750479849536</v>
+      <c r="H105" t="str">
+        <v>2013-07-05</v>
       </c>
       <c r="I105" t="str">
         <v>CALLE 18 S/N</v>
@@ -6621,8 +6621,8 @@
       <c r="G106" t="str">
         <v>humh4@hotmail.com</v>
       </c>
-      <c r="H106">
-        <v>25568.750479849536</v>
+      <c r="H106" t="str">
+        <v>2013-07-05</v>
       </c>
       <c r="I106" t="str">
         <v>CALLE 18 S/N</v>
@@ -6680,8 +6680,8 @@
       <c r="G107" t="str">
         <v>humh4@hotmail.com</v>
       </c>
-      <c r="H107">
-        <v>25568.750479849536</v>
+      <c r="H107" t="str">
+        <v>2013-07-05</v>
       </c>
       <c r="I107" t="str">
         <v>CALLE 18 S/N</v>
@@ -6739,8 +6739,8 @@
       <c r="G108" t="str">
         <v>humh4@hotmail.com</v>
       </c>
-      <c r="H108">
-        <v>25568.750479849536</v>
+      <c r="H108" t="str">
+        <v>2013-07-05</v>
       </c>
       <c r="I108" t="str">
         <v>CALLE 18 S/N</v>
@@ -6798,8 +6798,8 @@
       <c r="G109" t="str">
         <v>josebadz@outlook.com</v>
       </c>
-      <c r="H109">
-        <v>25568.750484652777</v>
+      <c r="H109" t="str">
+        <v>2014-08-24</v>
       </c>
       <c r="I109" t="str">
         <v>C. BENJAMIN ROMERO No. 64</v>
@@ -6857,8 +6857,8 @@
       <c r="G110" t="str">
         <v>josebadz@outlook.com</v>
       </c>
-      <c r="H110">
-        <v>25568.750484652777</v>
+      <c r="H110" t="str">
+        <v>2014-08-24</v>
       </c>
       <c r="I110" t="str">
         <v>C. BENJAMIN ROMERO No. 64</v>
@@ -6916,8 +6916,8 @@
       <c r="G111" t="str">
         <v>josebadz@outlook.com</v>
       </c>
-      <c r="H111">
-        <v>25568.750484652777</v>
+      <c r="H111" t="str">
+        <v>2014-08-24</v>
       </c>
       <c r="I111" t="str">
         <v>C. BENJAMIN ROMERO No. 64</v>
@@ -6975,8 +6975,8 @@
       <c r="G112" t="str">
         <v>josebadz@outlook.com</v>
       </c>
-      <c r="H112">
-        <v>25568.750484652777</v>
+      <c r="H112" t="str">
+        <v>2014-08-24</v>
       </c>
       <c r="I112" t="str">
         <v>C. BENJAMIN ROMERO No. 64</v>
@@ -7034,8 +7034,8 @@
       <c r="G113" t="str">
         <v>josebadz@outlook.com</v>
       </c>
-      <c r="H113">
-        <v>25568.750484652777</v>
+      <c r="H113" t="str">
+        <v>2014-08-24</v>
       </c>
       <c r="I113" t="str">
         <v>C. BENJAMIN ROMERO No. 64</v>
@@ -7093,8 +7093,8 @@
       <c r="G114" t="str">
         <v>josebadz@outlook.com</v>
       </c>
-      <c r="H114">
-        <v>25568.750484652777</v>
+      <c r="H114" t="str">
+        <v>2014-08-24</v>
       </c>
       <c r="I114" t="str">
         <v>C. BENJAMIN ROMERO No. 64</v>
@@ -7152,8 +7152,8 @@
       <c r="G115" t="str">
         <v>cudaosj@hotmail.com</v>
       </c>
-      <c r="H115">
-        <v>25568.750487118057</v>
+      <c r="H115" t="str">
+        <v>2015-03-24</v>
       </c>
       <c r="I115" t="str">
         <v>CALLE 60 No. 385 x 41 y 43</v>
@@ -7211,8 +7211,8 @@
       <c r="G116" t="str">
         <v>cudaosj@hotmail.com</v>
       </c>
-      <c r="H116">
-        <v>25568.750487118057</v>
+      <c r="H116" t="str">
+        <v>2015-03-24</v>
       </c>
       <c r="I116" t="str">
         <v>CALLE 60 No. 385 x 41 y 43</v>
@@ -7270,8 +7270,8 @@
       <c r="G117" t="str">
         <v>cudaosj@hotmail.com</v>
       </c>
-      <c r="H117">
-        <v>25568.750487118057</v>
+      <c r="H117" t="str">
+        <v>2015-03-24</v>
       </c>
       <c r="I117" t="str">
         <v>CALLE 60 No. 385 x 41 y 43</v>
@@ -7329,8 +7329,8 @@
       <c r="G118" t="str">
         <v>cudaosj@hotmail.com</v>
       </c>
-      <c r="H118">
-        <v>25568.750487118057</v>
+      <c r="H118" t="str">
+        <v>2015-03-24</v>
       </c>
       <c r="I118" t="str">
         <v>CALLE 60 No. 385 x 41 y 43</v>
@@ -7388,8 +7388,8 @@
       <c r="G119" t="str">
         <v>cudaosj@hotmail.com</v>
       </c>
-      <c r="H119">
-        <v>25568.750487118057</v>
+      <c r="H119" t="str">
+        <v>2015-03-24</v>
       </c>
       <c r="I119" t="str">
         <v>CALLE 60 No. 385 x 41 y 43</v>
@@ -7447,8 +7447,8 @@
       <c r="G120" t="str">
         <v>smunozam@gmail.com</v>
       </c>
-      <c r="H120">
-        <v>25568.750489351853</v>
+      <c r="H120" t="str">
+        <v>2015-10-04</v>
       </c>
       <c r="I120" t="str">
         <v>CALLE 26 No. 246 x 15 DEPTO. B</v>
@@ -7506,8 +7506,8 @@
       <c r="G121" t="str">
         <v>smunozam@gmail.com</v>
       </c>
-      <c r="H121">
-        <v>25568.750489351853</v>
+      <c r="H121" t="str">
+        <v>2015-10-04</v>
       </c>
       <c r="I121" t="str">
         <v>CALLE 26 No. 246 x 15 DEPTO. B</v>
@@ -7565,8 +7565,8 @@
       <c r="G122" t="str">
         <v>smunozam@gmail.com</v>
       </c>
-      <c r="H122">
-        <v>25568.750489351853</v>
+      <c r="H122" t="str">
+        <v>2015-10-04</v>
       </c>
       <c r="I122" t="str">
         <v>CALLE 26 No. 246 x 15 DEPTO. B</v>
@@ -7624,8 +7624,8 @@
       <c r="G123" t="str">
         <v>smunozam@gmail.com</v>
       </c>
-      <c r="H123">
-        <v>25568.750489351853</v>
+      <c r="H123" t="str">
+        <v>2015-10-04</v>
       </c>
       <c r="I123" t="str">
         <v>CALLE 26 No. 246 x 15 DEPTO. B</v>
@@ -7683,8 +7683,8 @@
       <c r="G124" t="str">
         <v>smunozam@gmail.com</v>
       </c>
-      <c r="H124">
-        <v>25568.750489351853</v>
+      <c r="H124" t="str">
+        <v>2015-10-04</v>
       </c>
       <c r="I124" t="str">
         <v>CALLE 26 No. 246 x 15 DEPTO. B</v>
@@ -7742,8 +7742,8 @@
       <c r="G125" t="str">
         <v>smunozam@gmail.com</v>
       </c>
-      <c r="H125">
-        <v>25568.750489351853</v>
+      <c r="H125" t="str">
+        <v>2015-10-04</v>
       </c>
       <c r="I125" t="str">
         <v>CALLE 26 No. 246 x 15 DEPTO. B</v>
@@ -7801,8 +7801,8 @@
       <c r="G126" t="str">
         <v>agm@galletasdonde.com</v>
       </c>
-      <c r="H126">
-        <v>25568.75049013889</v>
+      <c r="H126" t="str">
+        <v>2015-12-10</v>
       </c>
       <c r="I126" t="str">
         <v>CALLE 30 No. 275-A</v>
@@ -7860,8 +7860,8 @@
       <c r="G127" t="str">
         <v>agm@galletasdonde.com</v>
       </c>
-      <c r="H127">
-        <v>25568.75049013889</v>
+      <c r="H127" t="str">
+        <v>2015-12-10</v>
       </c>
       <c r="I127" t="str">
         <v>CALLE 30 No. 275-A</v>
@@ -7919,8 +7919,8 @@
       <c r="G128" t="str">
         <v>agm@galletasdonde.com</v>
       </c>
-      <c r="H128">
-        <v>25568.75049013889</v>
+      <c r="H128" t="str">
+        <v>2015-12-10</v>
       </c>
       <c r="I128" t="str">
         <v>CALLE 30 No. 275-A</v>
@@ -7978,8 +7978,8 @@
       <c r="G129" t="str">
         <v>agm@galletasdonde.com</v>
       </c>
-      <c r="H129">
-        <v>25568.75049013889</v>
+      <c r="H129" t="str">
+        <v>2015-12-10</v>
       </c>
       <c r="I129" t="str">
         <v>CALLE 30 No. 275-A</v>
@@ -8037,8 +8037,8 @@
       <c r="G130" t="str">
         <v>agm@galletasdonde.com</v>
       </c>
-      <c r="H130">
-        <v>25568.75049013889</v>
+      <c r="H130" t="str">
+        <v>2015-12-10</v>
       </c>
       <c r="I130" t="str">
         <v>CALLE 30 No. 275-A</v>
@@ -8096,8 +8096,8 @@
       <c r="G131" t="str">
         <v>agm@galletasdonde.com</v>
       </c>
-      <c r="H131">
-        <v>25568.75049013889</v>
+      <c r="H131" t="str">
+        <v>2015-12-10</v>
       </c>
       <c r="I131" t="str">
         <v>CALLE 30 No. 275-A</v>
@@ -8155,8 +8155,8 @@
       <c r="G132" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H132">
-        <v>25568.750491203704</v>
+      <c r="H132" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I132" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8214,8 +8214,8 @@
       <c r="G133" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H133">
-        <v>25568.750491203704</v>
+      <c r="H133" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I133" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8273,8 +8273,8 @@
       <c r="G134" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H134">
-        <v>25568.750491203704</v>
+      <c r="H134" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I134" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8332,8 +8332,8 @@
       <c r="G135" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H135">
-        <v>25568.750491203704</v>
+      <c r="H135" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I135" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8391,8 +8391,8 @@
       <c r="G136" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H136">
-        <v>25568.750491203704</v>
+      <c r="H136" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I136" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8450,8 +8450,8 @@
       <c r="G137" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H137">
-        <v>25568.750491203704</v>
+      <c r="H137" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I137" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8509,8 +8509,8 @@
       <c r="G138" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H138">
-        <v>25568.750491203704</v>
+      <c r="H138" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I138" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8568,8 +8568,8 @@
       <c r="G139" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H139">
-        <v>25568.750491203704</v>
+      <c r="H139" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I139" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8627,8 +8627,8 @@
       <c r="G140" t="str">
         <v>javier_ruzperaza@hotmail.com</v>
       </c>
-      <c r="H140">
-        <v>25568.750491203704</v>
+      <c r="H140" t="str">
+        <v>2016-03-11</v>
       </c>
       <c r="I140" t="str">
         <v>CALLE 17 No. 87 x 16 y 18</v>
@@ -8686,8 +8686,8 @@
       <c r="G141" t="str">
         <v>hanstb@gmail.com</v>
       </c>
-      <c r="H141">
-        <v>25568.750491192128</v>
+      <c r="H141" t="str">
+        <v>2016-03-10</v>
       </c>
       <c r="I141" t="str">
         <v>CALLE 41 No. 162 x 36-D y 38</v>
@@ -8745,8 +8745,8 @@
       <c r="G142" t="str">
         <v>hanstb@gmail.com</v>
       </c>
-      <c r="H142">
-        <v>25568.750491192128</v>
+      <c r="H142" t="str">
+        <v>2016-03-10</v>
       </c>
       <c r="I142" t="str">
         <v>CALLE 41 No. 162 x 36-D y 38</v>
@@ -8804,8 +8804,8 @@
       <c r="G143" t="str">
         <v>hanstb@gmail.com</v>
       </c>
-      <c r="H143">
-        <v>25568.750491192128</v>
+      <c r="H143" t="str">
+        <v>2016-03-10</v>
       </c>
       <c r="I143" t="str">
         <v>CALLE 41 No. 162 x 36-D y 38</v>
@@ -8863,8 +8863,8 @@
       <c r="G144" t="str">
         <v>hanstb@gmail.com</v>
       </c>
-      <c r="H144">
-        <v>25568.750491192128</v>
+      <c r="H144" t="str">
+        <v>2016-03-10</v>
       </c>
       <c r="I144" t="str">
         <v>CALLE 41 No. 162 x 36-D y 38</v>
@@ -8922,8 +8922,8 @@
       <c r="G145" t="str">
         <v>hanstb@gmail.com</v>
       </c>
-      <c r="H145">
-        <v>25568.750491192128</v>
+      <c r="H145" t="str">
+        <v>2016-03-10</v>
       </c>
       <c r="I145" t="str">
         <v>CALLE 41 No. 162 x 36-D y 38</v>
@@ -8981,8 +8981,8 @@
       <c r="G146" t="str">
         <v>hanstb@gmail.com</v>
       </c>
-      <c r="H146">
-        <v>25568.750491192128</v>
+      <c r="H146" t="str">
+        <v>2016-03-10</v>
       </c>
       <c r="I146" t="str">
         <v>CALLE 41 No. 162 x 36-D y 38</v>
@@ -9040,8 +9040,8 @@
       <c r="G147" t="str">
         <v>david_xolz@hotmail.com</v>
       </c>
-      <c r="H147">
-        <v>25568.75049152778</v>
+      <c r="H147" t="str">
+        <v>2016-04-09</v>
       </c>
       <c r="I147" t="str">
         <v>CALLE 29 No. 471 x 42 y 46-A</v>
@@ -9099,8 +9099,8 @@
       <c r="G148" t="str">
         <v>josegilbertohernandezcarrillo@gmail.com</v>
       </c>
-      <c r="H148">
-        <v>25568.750491898147</v>
+      <c r="H148" t="str">
+        <v>2016-05-11</v>
       </c>
       <c r="I148" t="str">
         <v>CALLE 2 No. 343 x 29 y 31</v>
@@ -9158,8 +9158,8 @@
       <c r="G149" t="str">
         <v>galvani@hotmail.com</v>
       </c>
-      <c r="H149">
-        <v>25568.750495069446</v>
+      <c r="H149" t="str">
+        <v>2017-05-16</v>
       </c>
       <c r="I149" t="str">
         <v>CALLE 31 No. 197 x 20 y 22</v>
@@ -9453,8 +9453,8 @@
       <c r="G154" t="str">
         <v>rafael-rivas-p@hotmail.com</v>
       </c>
-      <c r="H154">
-        <v>25568.750499108795</v>
+      <c r="H154" t="str">
+        <v>2018-01-23</v>
       </c>
       <c r="I154" t="str">
         <v>CALLE 12 No. 404-C x 15-A y 17 COL. DÍAZ ORDAZ</v>
@@ -9512,8 +9512,8 @@
       <c r="G155" t="str">
         <v>rafael-rivas-p@hotmail.com</v>
       </c>
-      <c r="H155">
-        <v>25568.750499108795</v>
+      <c r="H155" t="str">
+        <v>2018-01-23</v>
       </c>
       <c r="I155" t="str">
         <v>CALLE 12 No. 404-C x 15-A y 17 COL. DÍAZ ORDAZ</v>
@@ -9571,8 +9571,8 @@
       <c r="G156" t="str">
         <v>rafael-rivas-p@hotmail.com</v>
       </c>
-      <c r="H156">
-        <v>25568.750499108795</v>
+      <c r="H156" t="str">
+        <v>2018-01-23</v>
       </c>
       <c r="I156" t="str">
         <v>CALLE 12 No. 404-C x 15-A y 17 COL. DÍAZ ORDAZ</v>
@@ -9630,8 +9630,8 @@
       <c r="G157" t="str">
         <v>rafael-rivas-p@hotmail.com</v>
       </c>
-      <c r="H157">
-        <v>25568.750499108795</v>
+      <c r="H157" t="str">
+        <v>2018-01-23</v>
       </c>
       <c r="I157" t="str">
         <v>CALLE 12 No. 404-C x 15-A y 17 COL. DÍAZ ORDAZ</v>
@@ -9689,8 +9689,8 @@
       <c r="G158" t="str">
         <v>alejandrapintado@yahoo.com.mx</v>
       </c>
-      <c r="H158">
-        <v>25568.750499108795</v>
+      <c r="H158" t="str">
+        <v>2018-01-23</v>
       </c>
       <c r="I158" t="str">
         <v>CALLE 12 No. 404-C x 15-A y 17 COL. DÍAZ ORDAZ</v>
@@ -9748,8 +9748,8 @@
       <c r="G159" t="str">
         <v>tonysantacruz@hotmail.com</v>
       </c>
-      <c r="H159">
-        <v>25568.750507627316</v>
+      <c r="H159" t="str">
+        <v>2020-01-29</v>
       </c>
       <c r="I159" t="str">
         <v>CALLE 28 No. 168-A x 21-A y 21-B</v>
@@ -9807,8 +9807,8 @@
       <c r="G160" t="str">
         <v>marcotonyjr@hotmail.com</v>
       </c>
-      <c r="H160">
-        <v>25568.750507638888</v>
+      <c r="H160" t="str">
+        <v>2020-01-30</v>
       </c>
       <c r="I160" t="str">
         <v>CALLE 28 No. 168-A x 21-A y 21-B</v>
@@ -9866,8 +9866,8 @@
       <c r="G161" t="str">
         <v>chafi70@hotmail.com</v>
       </c>
-      <c r="H161">
-        <v>25568.7505078125</v>
+      <c r="H161" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I161" t="str">
         <v>C. 19-B No. 602 x 88</v>
@@ -9925,8 +9925,8 @@
       <c r="G162" t="str">
         <v>jcmaneo@hotmail.com</v>
       </c>
-      <c r="H162">
-        <v>25568.7505078125</v>
+      <c r="H162" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I162" t="str">
         <v>C. 59 No. 142 x 22</v>
@@ -9984,8 +9984,8 @@
       <c r="G163" t="str">
         <v>jcmaneo@hotmail.com</v>
       </c>
-      <c r="H163">
-        <v>25568.7505078125</v>
+      <c r="H163" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I163" t="str">
         <v>C. 59 No. 142 x 22</v>
@@ -10043,8 +10043,8 @@
       <c r="G164" t="str">
         <v>jcmaneo@hotmail.com</v>
       </c>
-      <c r="H164">
-        <v>25568.7505078125</v>
+      <c r="H164" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I164" t="str">
         <v>C. 59 No. 142 x 22</v>
@@ -10102,8 +10102,8 @@
       <c r="G165" t="str">
         <v>jcmaneo@hotmail.com</v>
       </c>
-      <c r="H165">
-        <v>25568.7505078125</v>
+      <c r="H165" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I165" t="str">
         <v>C. 59 No. 142 x 22</v>
@@ -10161,8 +10161,8 @@
       <c r="G166" t="str">
         <v>jcmaneo@hotmail.com</v>
       </c>
-      <c r="H166">
-        <v>25568.7505078125</v>
+      <c r="H166" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I166" t="str">
         <v>C. 59 No. 142 x 22</v>
@@ -10220,8 +10220,8 @@
       <c r="G167" t="str">
         <v>jcmaneo@hotmail.com</v>
       </c>
-      <c r="H167">
-        <v>25568.7505078125</v>
+      <c r="H167" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I167" t="str">
         <v>C. 59 No. 142 x 22</v>
@@ -10279,8 +10279,8 @@
       <c r="G168" t="str">
         <v>jcmaneo@hotmail.com</v>
       </c>
-      <c r="H168">
-        <v>25568.7505078125</v>
+      <c r="H168" t="str">
+        <v>2020-02-14</v>
       </c>
       <c r="I168" t="str">
         <v>C. 59 No. 142 x 22</v>
@@ -10338,8 +10338,8 @@
       <c r="G169" t="str">
         <v>tinosanchezf@yahoo.com.mx</v>
       </c>
-      <c r="H169">
-        <v>25568.750507928242</v>
+      <c r="H169" t="str">
+        <v>2020-02-24</v>
       </c>
       <c r="I169" t="str">
         <v>CALLE 20 No. 11399 x 29 y 29-B</v>
@@ -10397,8 +10397,8 @@
       <c r="G170" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H170">
-        <v>25568.750509421297</v>
+      <c r="H170" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I170" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10456,8 +10456,8 @@
       <c r="G171" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H171">
-        <v>25568.750509421297</v>
+      <c r="H171" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I171" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10515,8 +10515,8 @@
       <c r="G172" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H172">
-        <v>25568.750509421297</v>
+      <c r="H172" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I172" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10574,8 +10574,8 @@
       <c r="G173" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H173">
-        <v>25568.750509421297</v>
+      <c r="H173" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I173" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10633,8 +10633,8 @@
       <c r="G174" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H174">
-        <v>25568.750509421297</v>
+      <c r="H174" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I174" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10692,8 +10692,8 @@
       <c r="G175" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H175">
-        <v>25568.750509421297</v>
+      <c r="H175" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I175" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10751,8 +10751,8 @@
       <c r="G176" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H176">
-        <v>25568.750509421297</v>
+      <c r="H176" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I176" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10810,8 +10810,8 @@
       <c r="G177" t="str">
         <v>lalodenis23@hotmail.com</v>
       </c>
-      <c r="H177">
-        <v>25568.750509421297</v>
+      <c r="H177" t="str">
+        <v>2020-07-03</v>
       </c>
       <c r="I177" t="str">
         <v>CALLE 23-A x 16 y 18 No. 220</v>
@@ -10869,8 +10869,8 @@
       <c r="G178" t="str">
         <v>mayayuc3006@gmail.com</v>
       </c>
-      <c r="H178">
-        <v>25568.750510706017</v>
+      <c r="H178" t="str">
+        <v>2020-10-22</v>
       </c>
       <c r="I178" t="str">
         <v>CALLE 30-A No. 502-N x 69-A y 71</v>
@@ -10928,8 +10928,8 @@
       <c r="G179" t="str">
         <v>rodrigo.garcia.e@live.com.mx</v>
       </c>
-      <c r="H179">
-        <v>25568.75051181713</v>
+      <c r="H179" t="str">
+        <v>2021-01-25</v>
       </c>
       <c r="I179" t="str">
         <v>CALLE 13 No. 757 x 78 A</v>
@@ -10987,8 +10987,8 @@
       <c r="G180" t="str">
         <v>rodrigo.garcia.e@live.com.mx</v>
       </c>
-      <c r="H180">
-        <v>25568.75051181713</v>
+      <c r="H180" t="str">
+        <v>2021-01-25</v>
       </c>
       <c r="I180" t="str">
         <v>CALLE 13 No. 757 x 78 A</v>
@@ -11046,8 +11046,8 @@
       <c r="G181" t="str">
         <v>jretana@live.com.mx</v>
       </c>
-      <c r="H181">
-        <v>25568.75051193287</v>
+      <c r="H181" t="str">
+        <v>2021-02-04</v>
       </c>
       <c r="I181" t="str">
         <v>C. 27 No. 331 x 40 y 42</v>
@@ -11105,8 +11105,8 @@
       <c r="G182" t="str">
         <v>jretana@live.com.mx</v>
       </c>
-      <c r="H182">
-        <v>25568.75051193287</v>
+      <c r="H182" t="str">
+        <v>2021-02-04</v>
       </c>
       <c r="I182" t="str">
         <v>C. 27 No. 331 x 40 y 42</v>
@@ -11164,8 +11164,8 @@
       <c r="G183" t="str">
         <v>jretana@live.com.mx</v>
       </c>
-      <c r="H183">
-        <v>25568.75051193287</v>
+      <c r="H183" t="str">
+        <v>2021-02-04</v>
       </c>
       <c r="I183" t="str">
         <v>C. 27 No. 331 x 40 y 42</v>
@@ -11223,8 +11223,8 @@
       <c r="G184" t="str">
         <v>d@azarcorp.mx</v>
       </c>
-      <c r="H184">
-        <v>25568.75051355324</v>
+      <c r="H184" t="str">
+        <v>2021-06-25</v>
       </c>
       <c r="I184" t="str">
         <v>C. 12-A No. 61</v>
@@ -11282,8 +11282,8 @@
       <c r="G185" t="str">
         <v>quiquis77@hotmail.com</v>
       </c>
-      <c r="H185">
-        <v>25568.750516469907</v>
+      <c r="H185" t="str">
+        <v>2022-03-03</v>
       </c>
       <c r="I185" t="str">
         <v>C. 137 No. 1295</v>
@@ -11341,8 +11341,8 @@
       <c r="G186" t="str">
         <v>armando.pard@gmail.com</v>
       </c>
-      <c r="H186">
-        <v>25568.75051402778</v>
+      <c r="H186" t="str">
+        <v>2021-08-05</v>
       </c>
       <c r="I186" t="str">
         <v>C. 29 No. 216 x 4 y 6</v>
@@ -11400,8 +11400,8 @@
       <c r="G187" t="str">
         <v>valenciarojasjjesus@gmail.com</v>
       </c>
-      <c r="H187">
-        <v>25568.750518506946</v>
+      <c r="H187" t="str">
+        <v>2022-08-27</v>
       </c>
       <c r="I187" t="str">
         <v>C. 26 S/N x 53 y 55</v>
@@ -11459,8 +11459,8 @@
       <c r="G188" t="str">
         <v>valenciarojasjjesus@gmail.com</v>
       </c>
-      <c r="H188">
-        <v>25568.750518506946</v>
+      <c r="H188" t="str">
+        <v>2022-08-27</v>
       </c>
       <c r="I188" t="str">
         <v>C. 26 S/N x 53 y 55</v>
@@ -11518,8 +11518,8 @@
       <c r="G189" t="str">
         <v>valenciarojasjjesus@gmail.com</v>
       </c>
-      <c r="H189">
-        <v>25568.750518506946</v>
+      <c r="H189" t="str">
+        <v>2022-08-27</v>
       </c>
       <c r="I189" t="str">
         <v>C. 26 S/N x 53 y 55</v>
@@ -11577,8 +11577,8 @@
       <c r="G190" t="str">
         <v>brayerbyv@gmail.com</v>
       </c>
-      <c r="H190">
-        <v>25568.750522719907</v>
+      <c r="H190" t="str">
+        <v>2023-08-25</v>
       </c>
       <c r="I190" t="str">
         <v>C. 18-A x 31-D y 35</v>
@@ -11636,8 +11636,8 @@
       <c r="G191" t="str">
         <v>brayerbyv@gmail.com</v>
       </c>
-      <c r="H191">
-        <v>25568.750522719907</v>
+      <c r="H191" t="str">
+        <v>2023-08-25</v>
       </c>
       <c r="I191" t="str">
         <v>C. 18-A x 31-D y 35</v>
@@ -11695,8 +11695,8 @@
       <c r="G192" t="str">
         <v>brayerbyv@gmail.com</v>
       </c>
-      <c r="H192">
-        <v>25568.750522719907</v>
+      <c r="H192" t="str">
+        <v>2023-08-25</v>
       </c>
       <c r="I192" t="str">
         <v>C. 18-A x 31-D y 35</v>
@@ -11754,8 +11754,8 @@
       <c r="G193" t="str">
         <v>brayerbyv@gmail.com</v>
       </c>
-      <c r="H193">
-        <v>25568.750522719907</v>
+      <c r="H193" t="str">
+        <v>2023-08-25</v>
       </c>
       <c r="I193" t="str">
         <v>C. 18-A x 31-D y 35</v>
@@ -11813,8 +11813,8 @@
       <c r="G194" t="str">
         <v>rafle_30@hotmail.com</v>
       </c>
-      <c r="H194">
-        <v>25568.75052472222</v>
+      <c r="H194" t="str">
+        <v>2024-02-14</v>
       </c>
       <c r="I194" t="str">
         <v>C. 22C # 247 X 19</v>
@@ -11872,8 +11872,8 @@
       <c r="G195" t="str">
         <v>rafle_30@hotmail.com</v>
       </c>
-      <c r="H195">
-        <v>25568.75052472222</v>
+      <c r="H195" t="str">
+        <v>2024-02-14</v>
       </c>
       <c r="I195" t="str">
         <v>C. 22C # 247 X 19</v>
@@ -11931,8 +11931,8 @@
       <c r="G196" t="str">
         <v>rafle_30@hotmail.com</v>
       </c>
-      <c r="H196">
-        <v>25568.75052472222</v>
+      <c r="H196" t="str">
+        <v>2024-02-14</v>
       </c>
       <c r="I196" t="str">
         <v>C. 22C # 247 X 19</v>
@@ -11990,8 +11990,8 @@
       <c r="G197" t="str">
         <v>rafle_30@hotmail.com</v>
       </c>
-      <c r="H197">
-        <v>25568.75052472222</v>
+      <c r="H197" t="str">
+        <v>2024-02-14</v>
       </c>
       <c r="I197" t="str">
         <v>C. 22C # 247 X 19</v>
@@ -12049,8 +12049,8 @@
       <c r="G198" t="str">
         <v>rafle_30@hotmail.com</v>
       </c>
-      <c r="H198">
-        <v>25568.75052472222</v>
+      <c r="H198" t="str">
+        <v>2024-02-14</v>
       </c>
       <c r="I198" t="str">
         <v>C. 22C # 247 X 19</v>
@@ -12108,8 +12108,8 @@
       <c r="G199" t="str">
         <v>mjtzab@yahoo.com</v>
       </c>
-      <c r="H199">
-        <v>25568.750524837964</v>
+      <c r="H199" t="str">
+        <v>2024-02-24</v>
       </c>
       <c r="I199" t="str">
         <v>C. 103 # 624 X 142 Y 144</v>
@@ -12167,8 +12167,8 @@
       <c r="G200" t="str">
         <v>mjtzab@yahoo.com</v>
       </c>
-      <c r="H200">
-        <v>25568.750524837964</v>
+      <c r="H200" t="str">
+        <v>2024-02-24</v>
       </c>
       <c r="I200" t="str">
         <v>C. 103 # 624 X 142 Y 144</v>
@@ -12226,8 +12226,8 @@
       <c r="G201" t="str">
         <v>mjtzab@yahoo.com</v>
       </c>
-      <c r="H201">
-        <v>25568.750524837964</v>
+      <c r="H201" t="str">
+        <v>2024-02-24</v>
       </c>
       <c r="I201" t="str">
         <v>C. 103 # 624 X 142 Y 144</v>
@@ -12285,8 +12285,8 @@
       <c r="G202" t="str">
         <v>lic.arielparedescetina@hotmail.com</v>
       </c>
-      <c r="H202">
-        <v>25568.75052488426</v>
+      <c r="H202" t="str">
+        <v>2024-02-28</v>
       </c>
       <c r="I202" t="str">
         <v>CALLE 129 NO. 584 X 138 Y 140</v>
@@ -12344,8 +12344,8 @@
       <c r="G203" t="str">
         <v>lic.arielparedescetina@hotmail.com</v>
       </c>
-      <c r="H203">
-        <v>25568.75052488426</v>
+      <c r="H203" t="str">
+        <v>2024-02-28</v>
       </c>
       <c r="I203" t="str">
         <v>CALLE 129 NO. 584 X 138 Y 140</v>
@@ -12403,8 +12403,8 @@
       <c r="G204" t="str">
         <v>lic.arielparedescetina@hotmail.com</v>
       </c>
-      <c r="H204">
-        <v>25568.75052488426</v>
+      <c r="H204" t="str">
+        <v>2024-02-28</v>
       </c>
       <c r="I204" t="str">
         <v>CALLE 129 NO. 584 X 138 Y 140</v>
@@ -12462,8 +12462,8 @@
       <c r="G205" t="str">
         <v>dr.ricardocastillo@me.com</v>
       </c>
-      <c r="H205">
-        <v>25568.750525613425</v>
+      <c r="H205" t="str">
+        <v>2024-05-01</v>
       </c>
       <c r="I205" t="str">
         <v>CARR MÉRIDA PROGRESO KM 10.5 TABLAJE 19153</v>
@@ -12521,8 +12521,8 @@
       <c r="G206" t="str">
         <v>dr.ricardocastillo@me.com</v>
       </c>
-      <c r="H206">
-        <v>25568.750525613425</v>
+      <c r="H206" t="str">
+        <v>2024-05-01</v>
       </c>
       <c r="I206" t="str">
         <v>CARR MÉRIDA PROGRESO KM 10.5 TABLAJE 19153</v>
@@ -12580,8 +12580,8 @@
       <c r="G207" t="str">
         <v>cpedgardo_gomez@hotmail.com</v>
       </c>
-      <c r="H207">
-        <v>25568.750525613425</v>
+      <c r="H207" t="str">
+        <v>2024-05-01</v>
       </c>
       <c r="I207" t="str">
         <v>CALLE 7 NO 567 X 66 Y 68</v>
@@ -12624,8 +12624,8 @@
       <c r="G208" t="str">
         <v>lolita@concepthaus.mx</v>
       </c>
-      <c r="H208">
-        <v>25568.75052591435</v>
+      <c r="H208" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I208" t="str">
         <v>TABLAJE 13037 DEPTO 19 19 GRAND VIEW 6 Y 8</v>
@@ -12683,8 +12683,8 @@
       <c r="G209" t="str">
         <v>lolita@concepthaus.mx</v>
       </c>
-      <c r="H209">
-        <v>25568.75052591435</v>
+      <c r="H209" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I209" t="str">
         <v>TABLAJE 13037 DEPTO 19 19 GRAND VIEW 6 Y 8</v>
@@ -12742,8 +12742,8 @@
       <c r="G210" t="str">
         <v>lolita@concepthaus.mx</v>
       </c>
-      <c r="H210">
-        <v>25568.75052591435</v>
+      <c r="H210" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I210" t="str">
         <v>TABLAJE 13037 DEPTO 19 19 GRAND VIEW 6 Y 8</v>
@@ -12801,8 +12801,8 @@
       <c r="G211" t="str">
         <v>lolita@concepthaus.mx</v>
       </c>
-      <c r="H211">
-        <v>25568.75052591435</v>
+      <c r="H211" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I211" t="str">
         <v>TABLAJE 13037 DEPTO 19 19 GRAND VIEW 6 Y 8</v>
@@ -12860,8 +12860,8 @@
       <c r="G212" t="str">
         <v>lolita@concepthaus.mx</v>
       </c>
-      <c r="H212">
-        <v>25568.75052591435</v>
+      <c r="H212" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I212" t="str">
         <v>TABLAJE 13037 DEPTO 19 19 GRAND VIEW 6 Y 8</v>
@@ -12919,8 +12919,8 @@
       <c r="G213" t="str">
         <v>santiago100100@hotmail.com</v>
       </c>
-      <c r="H213">
-        <v>25568.75052591435</v>
+      <c r="H213" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I213" t="str">
         <v>CALLE 22 X 15 # 94-A</v>
@@ -12978,8 +12978,8 @@
       <c r="G214" t="str">
         <v>santiago100100@hotmail.com</v>
       </c>
-      <c r="H214">
-        <v>25568.75052591435</v>
+      <c r="H214" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I214" t="str">
         <v>CALLE 22 X 15 # 94-A</v>
@@ -13037,8 +13037,8 @@
       <c r="G215" t="str">
         <v>santiago100100@hotmail.com</v>
       </c>
-      <c r="H215">
-        <v>25568.75052591435</v>
+      <c r="H215" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I215" t="str">
         <v>CALLE 22 X 15 # 94-A</v>
@@ -13096,8 +13096,8 @@
       <c r="G216" t="str">
         <v>santiago100100@hotmail.com</v>
       </c>
-      <c r="H216">
-        <v>25568.75052591435</v>
+      <c r="H216" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I216" t="str">
         <v>CALLE 22 X 15 # 94-A</v>
@@ -13155,8 +13155,8 @@
       <c r="G217" t="str">
         <v>santiago100100@hotmail.com</v>
       </c>
-      <c r="H217">
-        <v>25568.75052591435</v>
+      <c r="H217" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I217" t="str">
         <v>CALLE 22 X 15 # 94-A</v>
@@ -13214,8 +13214,8 @@
       <c r="G218" t="str">
         <v>santiago100100@hotmail.com</v>
       </c>
-      <c r="H218">
-        <v>25568.75052591435</v>
+      <c r="H218" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I218" t="str">
         <v>CALLE 22 X 15 # 94-A</v>
@@ -13273,8 +13273,8 @@
       <c r="G219" t="str">
         <v>egpiccolo@gmail.com</v>
       </c>
-      <c r="H219">
-        <v>25568.75052591435</v>
+      <c r="H219" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I219" t="str">
         <v>C 40 POR 67 Y 69 234</v>
@@ -13332,8 +13332,8 @@
       <c r="G220" t="str">
         <v>egpiccolo@gmail.com</v>
       </c>
-      <c r="H220">
-        <v>25568.75052591435</v>
+      <c r="H220" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I220" t="str">
         <v>C 40 POR 67 Y 69 234</v>
@@ -13391,8 +13391,8 @@
       <c r="G221" t="str">
         <v>egpiccolo@gmail.com</v>
       </c>
-      <c r="H221">
-        <v>25568.75052591435</v>
+      <c r="H221" t="str">
+        <v>2024-05-27</v>
       </c>
       <c r="I221" t="str">
         <v>C 40 POR 67 Y 69 234</v>
@@ -13450,8 +13450,8 @@
       <c r="G222" t="str">
         <v>gfernandez63@gmail.com</v>
       </c>
-      <c r="H222">
-        <v>25568.75052658565</v>
+      <c r="H222" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I222" t="str">
         <v>Circuito Pablo García Oeste # 2 esquina con Eduardo Lavalle.</v>
@@ -13509,8 +13509,8 @@
       <c r="G223" t="str">
         <v>ridesquens@yahoo.com.mx</v>
       </c>
-      <c r="H223">
-        <v>25568.75052658565</v>
+      <c r="H223" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I223" t="str">
         <v>Calle 51-C # 643 x 72 y 72-A</v>
@@ -13568,8 +13568,8 @@
       <c r="G224" t="str">
         <v>ridesquens@yahoo.com.mx</v>
       </c>
-      <c r="H224">
-        <v>25568.75052658565</v>
+      <c r="H224" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I224" t="str">
         <v>Calle 51-C # 643 x 72 y 72-A</v>
@@ -13627,8 +13627,8 @@
       <c r="G225" t="str">
         <v>ridesquens@yahoo.com.mx</v>
       </c>
-      <c r="H225">
-        <v>25568.75052658565</v>
+      <c r="H225" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I225" t="str">
         <v>Calle 51-C # 643 x 72 y 72-A</v>
@@ -13686,8 +13686,8 @@
       <c r="G226" t="str">
         <v>ridesquens@yahoo.com.mx</v>
       </c>
-      <c r="H226">
-        <v>25568.75052658565</v>
+      <c r="H226" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I226" t="str">
         <v>Calle 51-C # 643 x 72 y 72-A</v>
@@ -13745,8 +13745,8 @@
       <c r="G227" t="str">
         <v>ridesquens@yahoo.com.mx</v>
       </c>
-      <c r="H227">
-        <v>25568.75052658565</v>
+      <c r="H227" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I227" t="str">
         <v>Calle 51-C # 643 x 72 y 72-A</v>
@@ -13804,8 +13804,8 @@
       <c r="G228" t="str">
         <v>ridesquens@yahoo.com.mx</v>
       </c>
-      <c r="H228">
-        <v>25568.75052658565</v>
+      <c r="H228" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I228" t="str">
         <v>Calle 51-C # 643 x 72 y 72-A</v>
@@ -13863,8 +13863,8 @@
       <c r="G229" t="str">
         <v>martinezasergio@hotmail.com</v>
       </c>
-      <c r="H229">
-        <v>25568.75052658565</v>
+      <c r="H229" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I229" t="str">
         <v>Calle 74 No. 629 x 37-A y 39</v>
@@ -13922,8 +13922,8 @@
       <c r="G230" t="str">
         <v>martinezasergio@hotmail.com</v>
       </c>
-      <c r="H230">
-        <v>25568.75052658565</v>
+      <c r="H230" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I230" t="str">
         <v>Calle 74 No. 629 x 37-A y 39</v>
@@ -13981,8 +13981,8 @@
       <c r="G231" t="str">
         <v>martinezasergio@hotmail.com</v>
       </c>
-      <c r="H231">
-        <v>25568.75052658565</v>
+      <c r="H231" t="str">
+        <v>2024-07-24</v>
       </c>
       <c r="I231" t="str">
         <v>Calle 74 No. 629 x 37-A y 39</v>
@@ -14040,8 +14040,8 @@
       <c r="G232" t="str">
         <v>arobert01@protonmail.com</v>
       </c>
-      <c r="H232">
-        <v>25568.750526909724</v>
+      <c r="H232" t="str">
+        <v>2024-08-21</v>
       </c>
       <c r="I232" t="str">
         <v>Calle 20A Núm 407 x 33 y 35.</v>
@@ -14099,8 +14099,8 @@
       <c r="G233" t="str">
         <v>arobert01@protonmail.com</v>
       </c>
-      <c r="H233">
-        <v>25568.750526909724</v>
+      <c r="H233" t="str">
+        <v>2024-08-21</v>
       </c>
       <c r="I233" t="str">
         <v>Calle 20A Núm 407 x 33 y 35.</v>
@@ -14158,8 +14158,8 @@
       <c r="G234" t="str">
         <v>arobert01@protonmail.com</v>
       </c>
-      <c r="H234">
-        <v>25568.750526909724</v>
+      <c r="H234" t="str">
+        <v>2024-08-21</v>
       </c>
       <c r="I234" t="str">
         <v>Calle 20A Núm 407 x 33 y 35.</v>
@@ -14217,8 +14217,8 @@
       <c r="G235" t="str">
         <v>olga.garcia@mayaseguridad.mx</v>
       </c>
-      <c r="H235">
-        <v>25568.75052710648</v>
+      <c r="H235" t="str">
+        <v>2024-09-07</v>
       </c>
       <c r="I235" t="str">
         <v>C. 81 112-2</v>
@@ -14276,8 +14276,8 @@
       <c r="G236" t="str">
         <v>gocaamal@hotmail.com</v>
       </c>
-      <c r="H236">
-        <v>25568.7505271875</v>
+      <c r="H236" t="str">
+        <v>2024-09-14</v>
       </c>
       <c r="I236" t="str">
         <v>CALLE 9 NÚM 681 X 74A y 74D</v>
@@ -14320,8 +14320,8 @@
       <c r="G237" t="str">
         <v>guidorcuevasabraham@gmail.com</v>
       </c>
-      <c r="H237">
-        <v>25568.750528101853</v>
+      <c r="H237" t="str">
+        <v>2024-12-02</v>
       </c>
       <c r="I237" t="str">
         <v>Calle 15 NÚM 314 x 32 y 34</v>
@@ -14379,8 +14379,8 @@
       <c r="G238" t="str">
         <v>guidorcuevasabraham@gmail.com</v>
       </c>
-      <c r="H238">
-        <v>25568.750528101853</v>
+      <c r="H238" t="str">
+        <v>2024-12-02</v>
       </c>
       <c r="I238" t="str">
         <v>Calle 15 NÚM 314 x 32 y 34</v>
@@ -14438,8 +14438,8 @@
       <c r="G239" t="str">
         <v>santiagorueda2@gmail.com</v>
       </c>
-      <c r="H239">
-        <v>25568.750528101853</v>
+      <c r="H239" t="str">
+        <v>2024-12-02</v>
       </c>
       <c r="I239" t="str">
         <v>C. 65 87</v>
@@ -14482,8 +14482,8 @@
       <c r="G240" t="str">
         <v>ivancabo@gmail.com</v>
       </c>
-      <c r="H240">
-        <v>25568.75052814815</v>
+      <c r="H240" t="str">
+        <v>2024-12-06</v>
       </c>
       <c r="I240" t="str">
         <v>C. 43 322 X 36 Y 36A</v>
@@ -14541,8 +14541,8 @@
       <c r="G241" t="str">
         <v>ivancabo@gmail.com</v>
       </c>
-      <c r="H241">
-        <v>25568.75052814815</v>
+      <c r="H241" t="str">
+        <v>2024-12-06</v>
       </c>
       <c r="I241" t="str">
         <v>C. 43 322 X 36 Y 36A</v>
@@ -14600,8 +14600,8 @@
       <c r="G242" t="str">
         <v>ivancabo@gmail.com</v>
       </c>
-      <c r="H242">
-        <v>25568.75052814815</v>
+      <c r="H242" t="str">
+        <v>2024-12-06</v>
       </c>
       <c r="I242" t="str">
         <v>C. 43 322 X 36 Y 36A</v>
@@ -14659,8 +14659,8 @@
       <c r="G243" t="str">
         <v>alejandro18sosa@gmail.com</v>
       </c>
-      <c r="H243">
-        <v>25568.75052826389</v>
+      <c r="H243" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I243" t="str">
         <v>C. 53 entre 58 y 60 NÚM. 425</v>
@@ -14703,8 +14703,8 @@
       <c r="G244" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="H244">
-        <v>25568.75052826389</v>
+      <c r="H244" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I244" t="str">
         <v>C. 46 480 X 33 Y 31 A</v>
@@ -14762,8 +14762,8 @@
       <c r="G245" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="H245">
-        <v>25568.75052826389</v>
+      <c r="H245" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I245" t="str">
         <v>C. 46 480 X 33 Y 31 A</v>
@@ -14821,8 +14821,8 @@
       <c r="G246" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="H246">
-        <v>25568.75052826389</v>
+      <c r="H246" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I246" t="str">
         <v>C. 46 480 X 33 Y 31 A</v>
@@ -14880,8 +14880,8 @@
       <c r="G247" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="H247">
-        <v>25568.75052826389</v>
+      <c r="H247" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I247" t="str">
         <v>C. 46 480 X 33 Y 31 A</v>
@@ -14939,8 +14939,8 @@
       <c r="G248" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="H248">
-        <v>25568.75052826389</v>
+      <c r="H248" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I248" t="str">
         <v>C. 46 480 X 33 Y 31 A</v>
@@ -14998,8 +14998,8 @@
       <c r="G249" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="H249">
-        <v>25568.75052826389</v>
+      <c r="H249" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I249" t="str">
         <v>C. 46 480 X 33 Y 31 A</v>
@@ -15057,8 +15057,8 @@
       <c r="G250" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="H250">
-        <v>25568.75052826389</v>
+      <c r="H250" t="str">
+        <v>2024-12-16</v>
       </c>
       <c r="I250" t="str">
         <v>C. 46 480 X 33 Y 31 A</v>
@@ -15116,8 +15116,8 @@
       <c r="G251" t="str">
         <v>squintal158@gmail.com</v>
       </c>
-      <c r="H251">
-        <v>25568.750529131943</v>
+      <c r="H251" t="str">
+        <v>2025-03-01</v>
       </c>
       <c r="I251" t="str">
         <v>CALLE 14 SIN NUMERO</v>
@@ -15175,8 +15175,8 @@
       <c r="G252" t="str">
         <v>squintal158@gmail.com</v>
       </c>
-      <c r="H252">
-        <v>25568.750529131943</v>
+      <c r="H252" t="str">
+        <v>2025-03-01</v>
       </c>
       <c r="I252" t="str">
         <v>CALLE 14 SIN NUMERO</v>
@@ -15234,8 +15234,8 @@
       <c r="G253" t="str">
         <v>squintal158@gmail.com</v>
       </c>
-      <c r="H253">
-        <v>25568.750529131943</v>
+      <c r="H253" t="str">
+        <v>2025-03-01</v>
       </c>
       <c r="I253" t="str">
         <v>CALLE 14 SIN NUMERO</v>
@@ -15293,8 +15293,8 @@
       <c r="G254" t="str">
         <v>atietzbabam@gmail.com</v>
       </c>
-      <c r="H254">
-        <v>25568.750529479166</v>
+      <c r="H254" t="str">
+        <v>2025-03-31</v>
       </c>
       <c r="I254" t="str">
         <v>C. 5-A DIAGONAL 239 X 18 Y 20</v>
@@ -15352,8 +15352,8 @@
       <c r="G255" t="str">
         <v>atietzbabam@gmail.com</v>
       </c>
-      <c r="H255">
-        <v>25568.750529479166</v>
+      <c r="H255" t="str">
+        <v>2025-03-31</v>
       </c>
       <c r="I255" t="str">
         <v>C. 5-A DIAGONAL 239 X 18 Y 20</v>
@@ -15411,8 +15411,8 @@
       <c r="G256" t="str">
         <v>atietzbabam@gmail.com</v>
       </c>
-      <c r="H256">
-        <v>25568.750529479166</v>
+      <c r="H256" t="str">
+        <v>2025-03-31</v>
       </c>
       <c r="I256" t="str">
         <v>C. 5-A DIAGONAL 239 X 18 Y 20</v>
@@ -15470,8 +15470,8 @@
       <c r="G257" t="str">
         <v>atietzbabam@gmail.com</v>
       </c>
-      <c r="H257">
-        <v>25568.750529479166</v>
+      <c r="H257" t="str">
+        <v>2025-03-31</v>
       </c>
       <c r="I257" t="str">
         <v>C. 5-A DIAGONAL 239 X 18 Y 20</v>
@@ -15529,8 +15529,8 @@
       <c r="G258" t="str">
         <v>atietzbabam@gmail.com</v>
       </c>
-      <c r="H258">
-        <v>25568.750529479166</v>
+      <c r="H258" t="str">
+        <v>2025-03-31</v>
       </c>
       <c r="I258" t="str">
         <v>C. 5-A DIAGONAL 239 X 18 Y 20</v>
@@ -15588,8 +15588,8 @@
       <c r="G259" t="str">
         <v>atietzbabam@gmail.com</v>
       </c>
-      <c r="H259">
-        <v>25568.750529479166</v>
+      <c r="H259" t="str">
+        <v>2025-03-31</v>
       </c>
       <c r="I259" t="str">
         <v>C. 5-A DIAGONAL 239 X 18 Y 20</v>
@@ -15647,8 +15647,8 @@
       <c r="G260" t="str">
         <v>atietzbabam@gmail.com</v>
       </c>
-      <c r="H260">
-        <v>25568.750529479166</v>
+      <c r="H260" t="str">
+        <v>2025-03-31</v>
       </c>
       <c r="I260" t="str">
         <v>C. 5-A DIAGONAL 239 X 18 Y 20</v>
@@ -15706,8 +15706,8 @@
       <c r="G261" t="str">
         <v>ttok09136@gmail.com</v>
       </c>
-      <c r="H261">
-        <v>25568.750529282406</v>
+      <c r="H261" t="str">
+        <v>2025-03-14</v>
       </c>
       <c r="I261" t="str">
         <v>Calle 35 SN INT. townhouse</v>
@@ -15750,8 +15750,8 @@
       <c r="G262" t="str">
         <v>fabian.sievers3548@gmail.com</v>
       </c>
-      <c r="H262">
-        <v>25568.75052982639</v>
+      <c r="H262" t="str">
+        <v>2025-04-30</v>
       </c>
       <c r="I262" t="str">
         <v>Calle 28 x 5 y 7 48-A</v>
@@ -15809,8 +15809,8 @@
       <c r="G263" t="str">
         <v>fabian.sievers3548@gmail.com</v>
       </c>
-      <c r="H263">
-        <v>25568.75052982639</v>
+      <c r="H263" t="str">
+        <v>2025-04-30</v>
       </c>
       <c r="I263" t="str">
         <v>Calle 28 x 5 y 7 48-A</v>
@@ -15868,8 +15868,8 @@
       <c r="G264" t="str">
         <v>fabian.sievers3548@gmail.com</v>
       </c>
-      <c r="H264">
-        <v>25568.75052982639</v>
+      <c r="H264" t="str">
+        <v>2025-04-30</v>
       </c>
       <c r="I264" t="str">
         <v>Calle 28 x 5 y 7 48-A</v>
@@ -15927,8 +15927,8 @@
       <c r="G265" t="str">
         <v>padilla_079@hotmail.com</v>
       </c>
-      <c r="H265">
-        <v>25568.750530185185</v>
+      <c r="H265" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I265" t="str">
         <v>Calle Tzolkin Num 48</v>
@@ -15986,8 +15986,8 @@
       <c r="G266" t="str">
         <v>padilla_079@hotmail.com</v>
       </c>
-      <c r="H266">
-        <v>25568.750530185185</v>
+      <c r="H266" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I266" t="str">
         <v>Calle Tzolkin Num 48</v>
@@ -16045,8 +16045,8 @@
       <c r="G267" t="str">
         <v>padilla_079@hotmail.com</v>
       </c>
-      <c r="H267">
-        <v>25568.750530185185</v>
+      <c r="H267" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I267" t="str">
         <v>Calle Tzolkin Num 48</v>
@@ -16104,8 +16104,8 @@
       <c r="G268" t="str">
         <v>padilla_079@hotmail.com</v>
       </c>
-      <c r="H268">
-        <v>25568.750530185185</v>
+      <c r="H268" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I268" t="str">
         <v>Calle Tzolkin Num 48</v>
@@ -16163,8 +16163,8 @@
       <c r="G269" t="str">
         <v>padilla_079@hotmail.com</v>
       </c>
-      <c r="H269">
-        <v>25568.750530185185</v>
+      <c r="H269" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I269" t="str">
         <v>Calle Tzolkin Num 48</v>
@@ -16222,8 +16222,8 @@
       <c r="G270" t="str">
         <v>padilla_079@hotmail.com</v>
       </c>
-      <c r="H270">
-        <v>25568.750530185185</v>
+      <c r="H270" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I270" t="str">
         <v>Calle Tzolkin Num 48</v>
@@ -16281,8 +16281,8 @@
       <c r="G271" t="str">
         <v>rsoberanis11@hotmail.com</v>
       </c>
-      <c r="H271">
-        <v>25568.750530185185</v>
+      <c r="H271" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I271" t="str">
         <v>Calle 23 S/N T.C. 50641</v>
@@ -16340,8 +16340,8 @@
       <c r="G272" t="str">
         <v>rsoberanis11@hotmail.com</v>
       </c>
-      <c r="H272">
-        <v>25568.750530185185</v>
+      <c r="H272" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I272" t="str">
         <v>Calle 23 S/N T.C. 50641</v>
@@ -16399,8 +16399,8 @@
       <c r="G273" t="str">
         <v>rsoberanis11@hotmail.com</v>
       </c>
-      <c r="H273">
-        <v>25568.750530185185</v>
+      <c r="H273" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I273" t="str">
         <v>Calle 23 S/N T.C. 50641</v>
@@ -16458,8 +16458,8 @@
       <c r="G274" t="str">
         <v>rsoberanis11@hotmail.com</v>
       </c>
-      <c r="H274">
-        <v>25568.750530185185</v>
+      <c r="H274" t="str">
+        <v>2025-05-31</v>
       </c>
       <c r="I274" t="str">
         <v>Calle 23 S/N T.C. 50641</v>
@@ -16517,8 +16517,8 @@
       <c r="G275" t="str">
         <v>rcervantes@live.com.mx</v>
       </c>
-      <c r="H275">
-        <v>25568.750530497684</v>
+      <c r="H275" t="str">
+        <v>2025-06-27</v>
       </c>
       <c r="I275" t="str">
         <v>C 13 POR 62 Y 64 655</v>
@@ -16561,8 +16561,8 @@
       <c r="G276" t="str">
         <v>richfer0304@gmail.com</v>
       </c>
-      <c r="H276">
-        <v>25568.750530833335</v>
+      <c r="H276" t="str">
+        <v>2025-07-26</v>
       </c>
       <c r="I276" t="str">
         <v>C. 37-A # 311 X 24</v>
@@ -16605,8 +16605,8 @@
       <c r="G277" t="str">
         <v>richfer1020@gmail.com</v>
       </c>
-      <c r="H277">
-        <v>25568.750530833335</v>
+      <c r="H277" t="str">
+        <v>2025-07-26</v>
       </c>
       <c r="I277" t="str">
         <v>C. 37-A # 311 X 24</v>
@@ -16664,8 +16664,8 @@
       <c r="G278" t="str">
         <v>licyaelromero@gmail.com</v>
       </c>
-      <c r="H278">
-        <v>25568.750531238427</v>
+      <c r="H278" t="str">
+        <v>2025-08-30</v>
       </c>
       <c r="I278" t="str">
         <v>Calle 111 No 514 x 132 y 134A</v>
@@ -16708,8 +16708,8 @@
       <c r="G279" t="str">
         <v>aimeegomez615@gmail.com</v>
       </c>
-      <c r="H279">
-        <v>25568.750532476854</v>
+      <c r="H279" t="str">
+        <v>2025-12-15</v>
       </c>
       <c r="I279" t="str">
         <v>C 63 D POR 88 TAB 42155</v>
@@ -16743,6 +16743,9 @@
       <c r="G280" t="str">
         <v>jrgardoni@gmail.com</v>
       </c>
+      <c r="H280" t="str">
+        <v>2021-12-14</v>
+      </c>
       <c r="N280" t="str">
         <v>PISTOLA</v>
       </c>
@@ -16775,6 +16778,9 @@
       <c r="G281" t="str">
         <v>jrgardoni@gmail.com</v>
       </c>
+      <c r="H281" t="str">
+        <v>2021-12-14</v>
+      </c>
       <c r="N281" t="str">
         <v>RIFLE</v>
       </c>
@@ -16807,6 +16813,9 @@
       <c r="G282" t="str">
         <v>jrgardoni@gmail.com</v>
       </c>
+      <c r="H282" t="str">
+        <v>2021-12-14</v>
+      </c>
       <c r="N282" t="str">
         <v>RIFLE</v>
       </c>
@@ -16839,6 +16848,9 @@
       <c r="G283" t="str">
         <v>jrgardoni@gmail.com</v>
       </c>
+      <c r="H283" t="str">
+        <v>2021-12-14</v>
+      </c>
       <c r="N283" t="str">
         <v>RIFLE</v>
       </c>
@@ -16871,6 +16883,9 @@
       <c r="G284" t="str">
         <v>jrgardoni@gmail.com</v>
       </c>
+      <c r="H284" t="str">
+        <v>2021-12-14</v>
+      </c>
       <c r="N284" t="str">
         <v>PISTOLA</v>
       </c>
@@ -16903,6 +16918,9 @@
       <c r="G285" t="str">
         <v>jrgardoni@gmail.com</v>
       </c>
+      <c r="H285" t="str">
+        <v>2021-12-14</v>
+      </c>
       <c r="N285" t="str">
         <v>PISTOLA</v>
       </c>
@@ -16935,6 +16953,9 @@
       <c r="G286" t="str">
         <v>jrgardoni@gmail.com</v>
       </c>
+      <c r="H286" t="str">
+        <v>2021-12-14</v>
+      </c>
       <c r="N286" t="str">
         <v>PISTOLA</v>
       </c>
@@ -16967,6 +16988,9 @@
       <c r="G287" t="str">
         <v>arechiga@jogarplastics.com</v>
       </c>
+      <c r="H287" t="str">
+        <v>2024-06-28</v>
+      </c>
       <c r="N287" t="str">
         <v>PISTOLA</v>
       </c>
@@ -16999,6 +17023,9 @@
       <c r="G288" t="str">
         <v>arechiga@jogarplastics.com</v>
       </c>
+      <c r="H288" t="str">
+        <v>2024-06-28</v>
+      </c>
       <c r="N288" t="str">
         <v>PISTOLA</v>
       </c>
@@ -17031,6 +17058,9 @@
       <c r="G289" t="str">
         <v>arechiga@jogarplastics.com</v>
       </c>
+      <c r="H289" t="str">
+        <v>2024-06-28</v>
+      </c>
       <c r="N289" t="str">
         <v>PISTOLA</v>
       </c>
@@ -17060,6 +17090,9 @@
       <c r="G290" t="str">
         <v>tinosanchezf@yahoo.com.mx</v>
       </c>
+      <c r="H290" t="str">
+        <v>2020-02-24</v>
+      </c>
       <c r="N290" t="str">
         <v>RIFLE</v>
       </c>
@@ -17089,6 +17122,9 @@
       <c r="G291" t="str">
         <v>tinosanchezf@yahoo.com.mx</v>
       </c>
+      <c r="H291" t="str">
+        <v>2020-02-24</v>
+      </c>
       <c r="N291" t="str">
         <v>PISTOLA</v>
       </c>
@@ -17118,6 +17154,9 @@
       <c r="G292" t="str">
         <v>tinosanchezf@yahoo.com.mx</v>
       </c>
+      <c r="H292" t="str">
+        <v>2020-02-24</v>
+      </c>
       <c r="N292" t="str">
         <v>PISTOLA</v>
       </c>
@@ -17146,6 +17185,9 @@
       </c>
       <c r="G293" t="str">
         <v>tinosanchezf@yahoo.com.mx</v>
+      </c>
+      <c r="H293" t="str">
+        <v>2020-02-24</v>
       </c>
       <c r="N293" t="str">
         <v>PISTOLA</v>

</xml_diff>

<commit_message>
fix: corregir fecha de ALTA de Roberto Madahuar a 2012-10-31
- Madahuar tenía fecha serializada (25568.750477002315)
- Corregida a fecha real: 2012-10-31 (31-Oct-2012)
- Verificada contra ANEXO A de diciembre 2025 (serial 41213)
- Email sincronizado: rmadahuar@cotexsa.com.mx
- Credencial: 115
- Teléfono: 9999473478
- Reportes regenerados
</commit_message>
<xml_diff>
--- a/data/referencias/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/data/referencias/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -6444,8 +6444,8 @@
       <c r="G103" t="str">
         <v>rmadahuar@cotexsa.com.mx</v>
       </c>
-      <c r="H103">
-        <v>25568.750477002315</v>
+      <c r="H103" t="str">
+        <v>2012-10-31</v>
       </c>
       <c r="I103" t="str">
         <v>CALLE 41 No. 199 x 18</v>
@@ -6503,8 +6503,8 @@
       <c r="G104" t="str">
         <v>rmadahuar@cotexsa.com.mx</v>
       </c>
-      <c r="H104">
-        <v>25568.750477002315</v>
+      <c r="H104" t="str">
+        <v>2012-10-31</v>
       </c>
       <c r="I104" t="str">
         <v>CALLE 41 No. 199 x 18</v>

</xml_diff>